<commit_message>
filtered out single spec char typos
</commit_message>
<xml_diff>
--- a/estimate-written.xlsx
+++ b/estimate-written.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <r>
       <t xml:space="preserve">PRESTIGIOUS AGENCY </t>
@@ -104,22 +104,25 @@
     <t>LENGTH</t>
   </si>
   <si>
-    <t>TYFC2216H</t>
-  </si>
-  <si>
-    <t>CGO MSE SSH Camping Multi Model APR 30</t>
-  </si>
-  <si>
-    <t>TYFC2217H</t>
-  </si>
-  <si>
-    <t>TYFC2218H</t>
-  </si>
-  <si>
-    <t>CGO MSE SSH Rotation Multi Model APR 15</t>
-  </si>
-  <si>
-    <t>TYFC2219H</t>
+    <t>ZYFP2089H</t>
+  </si>
+  <si>
+    <t>POINT MSE Activities 3.0 SUVs JCare</t>
+  </si>
+  <si>
+    <t>ZYFP2090H</t>
+  </si>
+  <si>
+    <t>JYFP2087H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v004 POINT MSE Activities 3.0 SUVs JCare </t>
+  </si>
+  <si>
+    <t>ZYFP2088</t>
+  </si>
+  <si>
+    <t>POINT MSE Camping Trucks JCare</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                 </t>
@@ -1275,7 +1278,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="33"/>
@@ -1305,7 +1308,7 @@
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
@@ -1417,27 +1420,27 @@
     </row>
     <row r="29" ht="30" customHeight="1" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
       <c r="G29" s="40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I29" s="40" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J29" s="40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K29" s="40"/>
       <c r="L29" s="41"/>
@@ -1452,13 +1455,13 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C31" s="24">
         <v>2185</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E31" s="43"/>
       <c r="F31" s="43"/>
@@ -1471,13 +1474,13 @@
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="24">
         <v>3762</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E32" s="47"/>
       <c r="F32" s="19"/>
@@ -1496,7 +1499,7 @@
         <v>863</v>
       </c>
       <c r="D33" s="43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
@@ -1509,13 +1512,13 @@
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C34" s="21">
         <v>2330</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
@@ -1528,13 +1531,13 @@
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C35" s="21">
         <v>136</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E35" s="49"/>
       <c r="F35" s="50"/>
@@ -1547,13 +1550,13 @@
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C36" s="24">
         <v>592</v>
       </c>
       <c r="D36" s="46" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E36" s="47"/>
       <c r="F36" s="19"/>
@@ -1568,13 +1571,13 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C37" s="21">
         <v>524</v>
       </c>
       <c r="D37" s="46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E37" s="47"/>
       <c r="F37" s="19"/>
@@ -1593,7 +1596,7 @@
         <v>696</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E38" s="43"/>
       <c r="F38" s="43"/>
@@ -1606,13 +1609,13 @@
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C39" s="24">
         <v>584</v>
       </c>
       <c r="D39" s="46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E39" s="47"/>
       <c r="F39" s="19"/>
@@ -1625,13 +1628,13 @@
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C40" s="24">
         <v>564</v>
       </c>
       <c r="D40" s="46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E40" s="49"/>
       <c r="F40" s="50"/>
@@ -1644,13 +1647,13 @@
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" s="24">
         <v>596</v>
       </c>
       <c r="D41" s="46" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E41" s="47"/>
       <c r="F41" s="19"/>
@@ -1663,13 +1666,13 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C42" s="21">
         <v>2326</v>
       </c>
       <c r="D42" s="46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E42" s="47"/>
       <c r="F42" s="19"/>
@@ -1688,7 +1691,7 @@
         <v>676</v>
       </c>
       <c r="D43" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E43" s="49"/>
       <c r="F43" s="50"/>
@@ -1707,12 +1710,12 @@
         <v>732</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E44" s="49"/>
       <c r="F44" s="50"/>
       <c r="G44" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H44" s="44"/>
       <c r="I44" s="44"/>
@@ -1728,7 +1731,7 @@
         <v>720</v>
       </c>
       <c r="D45" s="46" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E45" s="49"/>
       <c r="F45" s="50"/>
@@ -1747,7 +1750,7 @@
         <v>832</v>
       </c>
       <c r="D46" s="46" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E46" s="47"/>
       <c r="F46" s="19"/>
@@ -1760,13 +1763,13 @@
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C47" s="21">
         <v>520</v>
       </c>
       <c r="D47" s="46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E47" s="47"/>
       <c r="F47" s="19"/>
@@ -1779,13 +1782,13 @@
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C48" s="24">
         <v>400</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E48" s="43"/>
       <c r="F48" s="43"/>
@@ -1804,7 +1807,7 @@
         <v>737</v>
       </c>
       <c r="D49" s="46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E49" s="49"/>
       <c r="F49" s="50"/>
@@ -1823,7 +1826,7 @@
         <v>2437</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E50" s="43"/>
       <c r="F50" s="43"/>
@@ -1842,7 +1845,7 @@
         <v>2394</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E51" s="43"/>
       <c r="F51" s="43"/>
@@ -1855,13 +1858,13 @@
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C52" s="24">
         <v>2192</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E52" s="43"/>
       <c r="F52" s="43"/>
@@ -1880,7 +1883,7 @@
         <v>760</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E53" s="43"/>
       <c r="F53" s="43"/>
@@ -1899,7 +1902,7 @@
         <v>792</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E54" s="43"/>
       <c r="F54" s="43"/>
@@ -1918,7 +1921,7 @@
         <v>840</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E55" s="43"/>
       <c r="F55" s="43"/>
@@ -1931,13 +1934,13 @@
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C56" s="24">
         <v>500</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E56" s="43"/>
       <c r="F56" s="43"/>
@@ -1958,7 +1961,7 @@
         <v>768</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
@@ -1971,13 +1974,13 @@
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C58" s="21">
         <v>2322</v>
       </c>
       <c r="D58" s="46" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E58" s="47"/>
       <c r="F58" s="19"/>
@@ -2003,7 +2006,7 @@
     </row>
     <row r="60" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D60" s="43" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E60" s="43"/>
       <c r="F60" s="43"/>
@@ -2039,7 +2042,7 @@
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.25">
@@ -2058,7 +2061,7 @@
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="56"/>
       <c r="C64" s="57" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D64" s="58"/>
       <c r="E64" s="58"/>
@@ -2210,7 +2213,7 @@
       <c r="B76" s="63"/>
       <c r="C76" s="64"/>
       <c r="D76" s="64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E76" s="64"/>
       <c r="F76" s="64"/>
@@ -2226,7 +2229,7 @@
       <c r="C80" s="11"/>
       <c r="D80" s="11"/>
       <c r="E80" s="30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F80" s="31"/>
       <c r="G80" s="39"/>

</xml_diff>